<commit_message>
accepting numeric excel datetimes, Fixes #1
</commit_message>
<xml_diff>
--- a/excel_adapter_test.xlsx
+++ b/excel_adapter_test.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITWRLDC-4\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\CSharp_Projects\electron_dashboard_excel_adapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B505AA6-8594-4648-AD8B-9792750659E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E9FAF602-AB50-4132-81BC-CFD7CE8E09A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="AnotherSheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>col1</t>
   </si>
@@ -62,11 +61,14 @@
   <si>
     <t>Meas_D</t>
   </si>
+  <si>
+    <t>TimeCol2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,9 +98,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +415,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6807997-F2B7-45D7-BEDB-3DB1726C448D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1280,19 +1283,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CD96A3-2D2E-45D9-85B7-DFEAE5C64994}">
-  <dimension ref="A1:E50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1308,8 +1312,11 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43771.513888888891</v>
       </c>
@@ -1325,8 +1332,11 @@
       <c r="E2">
         <v>734</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2">
+        <v>43771.513888888891</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43771.51458333333</v>
       </c>
@@ -1342,8 +1352,11 @@
       <c r="E3">
         <v>703</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>43771.51458333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43771.515277662038</v>
       </c>
@@ -1359,8 +1372,11 @@
       <c r="E4">
         <v>757</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2">
+        <v>43771.515277662038</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43771.515972048612</v>
       </c>
@@ -1376,8 +1392,11 @@
       <c r="E5">
         <v>718</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2">
+        <v>43771.515972048612</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43771.516666435185</v>
       </c>
@@ -1393,8 +1412,11 @@
       <c r="E6">
         <v>617</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <v>43771.516666435185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43771.517360821759</v>
       </c>
@@ -1410,8 +1432,11 @@
       <c r="E7">
         <v>786</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="2">
+        <v>43771.517360821759</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43771.518055208333</v>
       </c>
@@ -1427,8 +1452,11 @@
       <c r="E8">
         <v>565</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="2">
+        <v>43771.518055208333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43771.518749594907</v>
       </c>
@@ -1444,8 +1472,11 @@
       <c r="E9">
         <v>504</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2">
+        <v>43771.518749594907</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43771.51944398148</v>
       </c>
@@ -1461,8 +1492,11 @@
       <c r="E10">
         <v>674</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2">
+        <v>43771.51944398148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43771.520138368054</v>
       </c>
@@ -1478,8 +1512,11 @@
       <c r="E11">
         <v>757</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2">
+        <v>43771.520138368054</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43771.520832754628</v>
       </c>
@@ -1495,8 +1532,11 @@
       <c r="E12">
         <v>659</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2">
+        <v>43771.520832754628</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43771.521527141202</v>
       </c>
@@ -1512,8 +1552,11 @@
       <c r="E13">
         <v>602</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2">
+        <v>43771.521527141202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43771.522221527775</v>
       </c>
@@ -1529,8 +1572,11 @@
       <c r="E14">
         <v>695</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="2">
+        <v>43771.522221527775</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43771.522915914349</v>
       </c>
@@ -1546,8 +1592,11 @@
       <c r="E15">
         <v>741</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="2">
+        <v>43771.522915914349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43771.523610300923</v>
       </c>
@@ -1563,8 +1612,11 @@
       <c r="E16">
         <v>723</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="2">
+        <v>43771.523610300923</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43771.524304687497</v>
       </c>
@@ -1580,8 +1632,11 @@
       <c r="E17">
         <v>686</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="2">
+        <v>43771.524304687497</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43771.524999074078</v>
       </c>
@@ -1597,8 +1652,11 @@
       <c r="E18">
         <v>504</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="2">
+        <v>43771.524999074078</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43771.525693460651</v>
       </c>
@@ -1614,8 +1672,11 @@
       <c r="E19">
         <v>743</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="2">
+        <v>43771.525693460651</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43771.526387847225</v>
       </c>
@@ -1631,8 +1692,11 @@
       <c r="E20">
         <v>738</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="2">
+        <v>43771.526387847225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43771.527082233799</v>
       </c>
@@ -1648,8 +1712,11 @@
       <c r="E21">
         <v>546</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="2">
+        <v>43771.527082233799</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43771.527776620373</v>
       </c>
@@ -1665,8 +1732,11 @@
       <c r="E22">
         <v>601</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="2">
+        <v>43771.527776620373</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43771.528471006946</v>
       </c>
@@ -1682,8 +1752,11 @@
       <c r="E23">
         <v>661</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="2">
+        <v>43771.528471006946</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43771.52916539352</v>
       </c>
@@ -1699,8 +1772,11 @@
       <c r="E24">
         <v>606</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="2">
+        <v>43771.52916539352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43771.529859780094</v>
       </c>
@@ -1716,8 +1792,11 @@
       <c r="E25">
         <v>725</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="2">
+        <v>43771.529859780094</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43771.530554166668</v>
       </c>
@@ -1733,8 +1812,11 @@
       <c r="E26">
         <v>581</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="2">
+        <v>43771.530554166668</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43771.531248553241</v>
       </c>
@@ -1750,8 +1832,11 @@
       <c r="E27">
         <v>788</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="2">
+        <v>43771.531248553241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43771.531942939815</v>
       </c>
@@ -1767,8 +1852,11 @@
       <c r="E28">
         <v>535</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="2">
+        <v>43771.531942939815</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43771.532637326389</v>
       </c>
@@ -1784,8 +1872,11 @@
       <c r="E29">
         <v>629</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="2">
+        <v>43771.532637326389</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43771.533331712963</v>
       </c>
@@ -1801,8 +1892,11 @@
       <c r="E30">
         <v>529</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="2">
+        <v>43771.533331712963</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43771.534026099536</v>
       </c>
@@ -1818,8 +1912,11 @@
       <c r="E31">
         <v>619</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="2">
+        <v>43771.534026099536</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43771.53472048611</v>
       </c>
@@ -1835,8 +1932,11 @@
       <c r="E32">
         <v>599</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="2">
+        <v>43771.53472048611</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43771.535414872684</v>
       </c>
@@ -1852,8 +1952,11 @@
       <c r="E33">
         <v>620</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="2">
+        <v>43771.535414872684</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43771.536109259258</v>
       </c>
@@ -1869,8 +1972,11 @@
       <c r="E34">
         <v>711</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="2">
+        <v>43771.536109259258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43771.536803645831</v>
       </c>
@@ -1886,8 +1992,11 @@
       <c r="E35">
         <v>743</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="2">
+        <v>43771.536803645831</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43771.537498032405</v>
       </c>
@@ -1903,8 +2012,11 @@
       <c r="E36">
         <v>650</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="2">
+        <v>43771.537498032405</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43771.538192418979</v>
       </c>
@@ -1920,8 +2032,11 @@
       <c r="E37">
         <v>514</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="2">
+        <v>43771.538192418979</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43771.538886805552</v>
       </c>
@@ -1937,8 +2052,11 @@
       <c r="E38">
         <v>700</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="2">
+        <v>43771.538886805552</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43771.539581192126</v>
       </c>
@@ -1954,8 +2072,11 @@
       <c r="E39">
         <v>573</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="2">
+        <v>43771.539581192126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43771.540275578707</v>
       </c>
@@ -1971,8 +2092,11 @@
       <c r="E40">
         <v>591</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="2">
+        <v>43771.540275578707</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43771.540969965281</v>
       </c>
@@ -1988,8 +2112,11 @@
       <c r="E41">
         <v>757</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="2">
+        <v>43771.540969965281</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43771.541664351855</v>
       </c>
@@ -2005,8 +2132,11 @@
       <c r="E42">
         <v>564</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="2">
+        <v>43771.541664351855</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43771.542358738428</v>
       </c>
@@ -2022,8 +2152,11 @@
       <c r="E43">
         <v>695</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="2">
+        <v>43771.542358738428</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43771.543053125002</v>
       </c>
@@ -2039,8 +2172,11 @@
       <c r="E44">
         <v>526</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="2">
+        <v>43771.543053125002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43771.543747511576</v>
       </c>
@@ -2056,8 +2192,11 @@
       <c r="E45">
         <v>574</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="2">
+        <v>43771.543747511576</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43771.54444189815</v>
       </c>
@@ -2073,8 +2212,11 @@
       <c r="E46">
         <v>710</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="2">
+        <v>43771.54444189815</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43771.545136284723</v>
       </c>
@@ -2090,8 +2232,11 @@
       <c r="E47">
         <v>687</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="2">
+        <v>43771.545136284723</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43771.545830671297</v>
       </c>
@@ -2107,8 +2252,11 @@
       <c r="E48">
         <v>620</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="2">
+        <v>43771.545830671297</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43771.546525057871</v>
       </c>
@@ -2124,8 +2272,11 @@
       <c r="E49">
         <v>652</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="2">
+        <v>43771.546525057871</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43771.547219444445</v>
       </c>
@@ -2140,6 +2291,9 @@
       </c>
       <c r="E50">
         <v>792</v>
+      </c>
+      <c r="F50" s="2">
+        <v>43771.547219444445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>